<commit_message>
Find the Duplicate Number
</commit_message>
<xml_diff>
--- a/Premraj DSA Practice list.xlsx
+++ b/Premraj DSA Practice list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Tutorial\Problem Practices\Practice-DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D98265DB-DCFE-4FA6-9789-E19D2388D145}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C24E58E-1523-46DF-9946-06730B567B73}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1834,7 +1834,7 @@
   <dimension ref="A1:D1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2009,8 +2009,8 @@
       <c r="B16" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="12" t="s">
-        <v>12</v>
+      <c r="C16" s="7" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Running Sum of 1d Array
</commit_message>
<xml_diff>
--- a/Premraj DSA Practice list.xlsx
+++ b/Premraj DSA Practice list.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Tutorial\Problem Practices\Practice-DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C24E58E-1523-46DF-9946-06730B567B73}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52E61304-E0EE-4E2F-BFB8-69A806D5CACB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1834,7 +1834,7 @@
   <dimension ref="A1:D1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2031,8 +2031,8 @@
       <c r="B18" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="12" t="s">
-        <v>12</v>
+      <c r="C18" s="7" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Maximum Subarray (Kaden's Algorithm)
</commit_message>
<xml_diff>
--- a/Premraj DSA Practice list.xlsx
+++ b/Premraj DSA Practice list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Tutorial\Problem Practices\Practice-DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52E61304-E0EE-4E2F-BFB8-69A806D5CACB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB636DDC-D093-4ABD-A223-9DD1EE38DF72}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1834,7 +1834,7 @@
   <dimension ref="A1:D1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1918,8 +1918,8 @@
       <c r="B8" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="7" t="s">
-        <v>6</v>
+      <c r="C8" s="19" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>